<commit_message>
Add test scenarios, adjust python script and readme
</commit_message>
<xml_diff>
--- a/data/restful_booker_test_cases.xlsx
+++ b/data/restful_booker_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magda\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\restful-booker-test-cases\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABC4266B-AC54-4232-8077-77C8C476CDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0338FF-C465-4CBB-8AB7-BB04DEC1EC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B791E2F-D378-46E5-AF64-E91401ACDD1C}"/>
   </bookViews>
@@ -86,21 +86,16 @@
     <t>Currently, the response code is 200 OK.</t>
   </si>
   <si>
-    <t>1. Send API Request to the /auth endpoint.
-In the request, provide the username and password from the preconditions.</t>
-  </si>
-  <si>
-    <t>1. Response status is 200 OK.
-A token is generated.</t>
-  </si>
-  <si>
-    <t>1. Send API Request to the /auth endpoint.
-In the request, provide an invalid username and password.</t>
-  </si>
-  <si>
-    <t>⚠️ Documentation update required.
-👉 Rest API best practices
-* Response status is 401 Unauthorized for an invalid token.</t>
+    <t>1. Send API Request to the /auth endpoint.&lt;br/&gt; In the request, provide the username and password from the preconditions.</t>
+  </si>
+  <si>
+    <t>1. Response status is 200 OK.&lt;br/&gt;A token is generated.</t>
+  </si>
+  <si>
+    <t>1. Send API Request to the /auth endpoint.&lt;/br&gt;In the request, provide an invalid username and password.</t>
+  </si>
+  <si>
+    <t>⚠️ Documentation update required.&lt;/br&gt;👉 Rest API best practices&lt;/br&gt; * Response status is 401 Unauthorized for an invalid token.</t>
   </si>
 </sst>
 </file>
@@ -136,12 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -476,89 +470,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AA0928-6B48-4DE0-B8A8-20FEB99054DB}">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="61.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="111.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="111.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>